<commit_message>
Update elements and start designing
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pbpost\goodmanjurors\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,45 +19,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="13">
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>race</t>
-  </si>
-  <si>
-    <t>q1</t>
-  </si>
-  <si>
-    <t>q2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="27">
   <si>
     <t>no</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>white</t>
-  </si>
-  <si>
-    <t>black</t>
-  </si>
-  <si>
-    <t>hispanic</t>
-  </si>
-  <si>
-    <t>asian</t>
-  </si>
-  <si>
-    <t>yes</t>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Hispanic</t>
+  </si>
+  <si>
+    <t>priorjury</t>
+  </si>
+  <si>
+    <t>lawenforcement</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>witness</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>victim</t>
+  </si>
+  <si>
+    <t>arrested</t>
+  </si>
+  <si>
+    <t>lawsuit</t>
+  </si>
+  <si>
+    <t>claims</t>
+  </si>
+  <si>
+    <t>claimAgainst</t>
+  </si>
+  <si>
+    <t>Civil</t>
+  </si>
+  <si>
+    <t>Criminal</t>
+  </si>
+  <si>
+    <t>marital</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>Divorced</t>
+  </si>
+  <si>
+    <t>Widow(er)</t>
   </si>
 </sst>
 </file>
@@ -98,8 +135,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,7 +412,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -380,35 +420,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -416,19 +482,40 @@
         <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -436,19 +523,40 @@
         <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -456,19 +564,40 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -476,19 +605,40 @@
         <v>65</v>
       </c>
       <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -496,19 +646,40 @@
         <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -516,19 +687,40 @@
         <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -536,19 +728,40 @@
         <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -556,19 +769,40 @@
         <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -576,16 +810,37 @@
         <v>76</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>